<commit_message>
Adding PCBWAY Quotation, Editted the RAW FILE for BOM and added tab for parts that need to be ordered, parts that are not assembled by the PCBA manufacturer.
</commit_message>
<xml_diff>
--- a/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
+++ b/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PCBa_KRAKEKiCad6_250128_1359" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,6 +14,7 @@
     <sheet name="posPCBWAY" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="BOM jlcpcb" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="CPL JLCPCB" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="amazon" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2372,16 +2373,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2393,15 +2394,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2578,8 +2570,8 @@
   </sheetPr>
   <dimension ref="A1:W274"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2594,7 +2586,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="9.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="1" width="9.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25884,20 +25878,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="8" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>666</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>667</v>
       </c>
     </row>
@@ -28727,13 +28721,13 @@
   </sheetPr>
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="8" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32841,6 +32835,866 @@
       </c>
       <c r="E187" s="1" t="n">
         <f aca="false">posRAW!F187</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.31"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B213</f>
+        <v>Qty</v>
+      </c>
+      <c r="B1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C213</f>
+        <v>Reference(s)</v>
+      </c>
+      <c r="C1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D213</f>
+        <v>Value</v>
+      </c>
+      <c r="D1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G213</f>
+        <v>Datasheet</v>
+      </c>
+      <c r="E1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N213</f>
+        <v>Description</v>
+      </c>
+      <c r="F1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P213</f>
+        <v>Distributor 1</v>
+      </c>
+      <c r="G1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q213</f>
+        <v>Distributor 1 PN</v>
+      </c>
+      <c r="H1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R213</f>
+        <v>Distributor 2</v>
+      </c>
+      <c r="I1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S213</f>
+        <v>Distributor 2 PN</v>
+      </c>
+      <c r="J1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U213</f>
+        <v>MPN</v>
+      </c>
+      <c r="K1" s="10" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V213</f>
+        <v>Manufacturer</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B214</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C214</f>
+        <v>BZ601</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D214</f>
+        <v>Speaker</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G214</f>
+        <v>~</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N214</f>
+        <v>8 Ohm 2W Speaker 8ohm Round 28mm Loud Speakers Compatible with Small Loudspeaker Audio MP3 MP4 Player Speaker (with Terminal)</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P214</f>
+        <v>Amazon</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q214</f>
+        <v>https://www.amazon.com/dp/B0DCTL83H6</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R214</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S214</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U214</f>
+        <v>ZGW-1</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V214</f>
+        <v>	YFUSET</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B215</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C215</f>
+        <v>J603</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D215</f>
+        <v>DFPlayermini</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G215</f>
+        <v>https://image.dfrobot.com/image/data/DFR0299/DFPlayer%20Mini%20Manul.pdf</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N215</f>
+        <v>Mini MP3 Player</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P215</f>
+        <v>Amazon</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q215</f>
+        <v>Amazon</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R215</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S215</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U215</f>
+        <v>https://www.amazon.com/dp/B089D5NLW1</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V215</f>
+        <v>DFROBOT</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B216</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C216</f>
+        <v>J701</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D216</f>
+        <v>DE9_Receptacle_MountingHoles</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G216</f>
+        <v> ~</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N216</f>
+        <v>DB9 Male and Female D-Sub Solder Type Connector</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P216</f>
+        <v>Amazon</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q216</f>
+        <v>Amazon</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R216</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S216</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U216</f>
+        <v>https://www.amazon.com/Pc-Accessories-Connectors-Connector-20-Pack/dp/B014IVD7L0/ref=sr_1_1</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V216</f>
+        <v>Connectors Pro</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B217</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C217</f>
+        <v>SD601</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D217</f>
+        <v>Micro_SD_Card_16GB_DFPLAYER</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G217</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N217</f>
+        <v>SanDisk Flash 16 GB SDHC Flash Memory Card SDSDB-016G </v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P217</f>
+        <v>Amazon</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q217</f>
+        <v>https://www.amazon.com/SanDisk-Flash-Memory-SDSDB-016G-Change/dp/B001W1BSM0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R217</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S217</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U217</f>
+        <v>SDSDB-016G-E11</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V217</f>
+        <v>	SanDisk</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B218</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C218</f>
+        <v>D105</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D218</f>
+        <v>LED_T1.75_CLEAR_RED</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G218</f>
+        <v>http://optoelectronics.liteon.com/upload/download/DS20-2005-253/LTW-2R3D7.pdf</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N218</f>
+        <v>LED RED CLEAR T-1 3/4 T/H</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P218</f>
+        <v>DigiKey</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q218</f>
+        <v>160-1682-ND</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R218</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S218</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U218</f>
+        <v>LTL2R3KEK</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V218</f>
+        <v>Lite-On Inc.</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B219</f>
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C219</f>
+        <v>D201, D202, D203, D204, D205</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D219</f>
+        <v>LED_T1.75_CLEAR_WHITE</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G219</f>
+        <v>http://optoelectronics.liteon.com/upload/download/DS20-2005-253/LTW-2R3D7.pdf</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N219</f>
+        <v>LED WHITE CLEAR T-1 3/4 T/H</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P219</f>
+        <v>DigiKey</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q219</f>
+        <v>160-1772-ND</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R219</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S219</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U219</f>
+        <v>LTW-2R3D7</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V219</f>
+        <v>Lite-On Inc.</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B220</f>
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C220</f>
+        <v>MF403, MF406, MF409, MF412</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D220</f>
+        <v>Nut_4-40_0.1875</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G220</f>
+        <v>https://www.keyelco.com/userAssets/file/M65p135.pdf</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N220</f>
+        <v>#4-40 Hex Nut 0.187" (4.75mm) 3/16" Steel</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P220</f>
+        <v>DigiKey</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q220</f>
+        <v>36-4694-ND</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R220</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S220</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U220</f>
+        <v>4694</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V220</f>
+        <v>Keystone Electronics</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B221</f>
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C221</f>
+        <v>R106, R107, R306, R308</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D221</f>
+        <v>DNI</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G221</f>
+        <v>~</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N221</f>
+        <v>DNI</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P221</f>
+        <v>DNI</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q221</f>
+        <v>DNI</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R221</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S221</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U221</f>
+        <v>DNI</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V221</f>
+        <v>TyoHM</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B222</f>
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C222</f>
+        <v>U302</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D222</f>
+        <v>LCD_20x4_Character-GPAD_SCH_LIB</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G222</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N222</f>
+        <v>2004 LCD Display Module Character 20x4 Blacklight Gray Yellow Blue</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P222</f>
+        <v>eBay   Aliexpress</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q222</f>
+        <v>403534100457</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R222</f>
+        <v>Amazon  / Aliexpress</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S222</f>
+        <v>https://www.amazon.com/GeeekPi-Interface-Adapter-Backlight-Raspberry/dp/B07QLRD3TM/ref=sr_1_2 /  https://www.aliexpress.com/item/3256803213374992.html</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U222</f>
+        <v>https://www.ebay.com/itm/403534100457</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V222</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B268</f>
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C268</f>
+        <v>MF401, MF404, MF407, MF410</v>
+      </c>
+      <c r="C17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D268</f>
+        <v>Screw_4-40_0.375_Phillips</v>
+      </c>
+      <c r="D17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G268</f>
+        <v>https://www.mcmaster.com/catalog/128/3306</v>
+      </c>
+      <c r="E17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N268</f>
+        <v>Zinc-Plated Steel Pan Head Phillips Screw, 4-40 Thread, 3/8" Long</v>
+      </c>
+      <c r="F17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P268</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="G17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q268</f>
+        <v>90272A108</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R268</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S268</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U268</f>
+        <v>90272A108</v>
+      </c>
+      <c r="K17" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V268</f>
+        <v>McMaster-Carr</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B269</f>
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C269</f>
+        <v>MF402, MF405, MF408, MF411</v>
+      </c>
+      <c r="C18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D269</f>
+        <v>Spacer_0.0182x0.125 inch</v>
+      </c>
+      <c r="D18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G269</f>
+        <v>https://www.mcmaster.com/catalog/128/3306</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N269</f>
+        <v>Off-White Nylon Unthreaded Spacer, 0.1875" OD, 1/8" Long, for Number 4 Screw Size</v>
+      </c>
+      <c r="F18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P269</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="G18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q269</f>
+        <v>94639A702</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R269</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S269</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U269</f>
+        <v>94639A702</v>
+      </c>
+      <c r="K18" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V269</f>
+        <v>McMaster-Carr</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B270</f>
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C270</f>
+        <v>H101, H102, H103, H104</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D270</f>
+        <v>MountingHole_Pad_3.5mm</v>
+      </c>
+      <c r="D20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G270</f>
+        <v>~</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N270</f>
+        <v>MountingHole_Pad_3.5mm</v>
+      </c>
+      <c r="F20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P270</f>
+        <v>NA</v>
+      </c>
+      <c r="G20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q270</f>
+        <v>NA</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R270</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S270</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U270</f>
+        <v>NA</v>
+      </c>
+      <c r="K20" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V270</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B271</f>
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C271</f>
+        <v>MF103, MF601, MF602, MF603, MF604, MF605</v>
+      </c>
+      <c r="C21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D271</f>
+        <v>U_Box_V104_General_Alarm_Device_LED_Standoff</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G271</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N271</f>
+        <v>NA</v>
+      </c>
+      <c r="F21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P271</f>
+        <v>NA</v>
+      </c>
+      <c r="G21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q271</f>
+        <v>NA</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R271</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S271</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U271</f>
+        <v>NA</v>
+      </c>
+      <c r="K21" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V271</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B272</f>
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C272</f>
+        <v>T101, T102, T103</v>
+      </c>
+      <c r="C22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D272</f>
+        <v>ToolingHole_Pad_1.152mm</v>
+      </c>
+      <c r="D22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G272</f>
+        <v>~</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N272</f>
+        <v>ToolingHole_Pad_1.152mm</v>
+      </c>
+      <c r="F22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P272</f>
+        <v>NA</v>
+      </c>
+      <c r="G22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q272</f>
+        <v>NA</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R272</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S272</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U272</f>
+        <v>NA</v>
+      </c>
+      <c r="K22" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V272</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B273</f>
+        <v>1</v>
+      </c>
+      <c r="B24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C273</f>
+        <v>MF801</v>
+      </c>
+      <c r="C24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D273</f>
+        <v>ENCLOSURE_KRAKE_VER1</v>
+      </c>
+      <c r="D24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G273</f>
+        <v>https://www.mcmaster.com/catalog/128/3306</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N273</f>
+        <v>NA</v>
+      </c>
+      <c r="F24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P273</f>
+        <v>PublicInvention</v>
+      </c>
+      <c r="G24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q273</f>
+        <v>ENCLOSURE_KRAKE_VER1</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R273</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S273</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U273</f>
+        <v>NA</v>
+      </c>
+      <c r="K24" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V273</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B274</f>
+        <v>1</v>
+      </c>
+      <c r="B25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C274</f>
+        <v>MF802</v>
+      </c>
+      <c r="C25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D274</f>
+        <v>PCB_KRAKE_VER1</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G274</f>
+        <v>Gerbers2501181555.zip</v>
+      </c>
+      <c r="E25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N274</f>
+        <v>PCB for KRAKE Version 1</v>
+      </c>
+      <c r="F25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P274</f>
+        <v>PublicInvention</v>
+      </c>
+      <c r="G25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q274</f>
+        <v>PCB_KRAKE_V1</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R274</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S274</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="0" t="str">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U274</f>
+        <v>Gerbers2501181555.zip</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V274</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B275</f>
+        <v>0</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C275</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D275</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G275</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N275</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P275</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q275</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R275</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S275</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U275</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V275</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BO and Parts list as of 7th of feb 2025.
</commit_message>
<xml_diff>
--- a/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
+++ b/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
@@ -32856,8 +32856,8 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adding Amazon order details.
</commit_message>
<xml_diff>
--- a/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
+++ b/PCBa_KRAKE/PCBa_KRAKEKiCad6_250128_1359.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3866" uniqueCount="673">
   <si>
     <t xml:space="preserve">Source:</t>
   </si>
@@ -2197,16 +2197,20 @@
   <si>
     <t xml:space="preserve">Rotation</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/gp/product/B07Y2YKYRS/ref=ox_sc_act_title_1?smid=A39S0U3UP1U7UG&amp;th=1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2278,6 +2282,13 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2340,7 +2351,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2365,7 +2376,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2381,7 +2392,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -32854,20 +32869,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="4.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="13.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32917,788 +32936,514 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B214</f>
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="str">
+      <c r="B3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C214</f>
         <v>BZ601</v>
       </c>
-      <c r="C3" s="0" t="str">
+      <c r="C3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D214</f>
         <v>Speaker</v>
       </c>
-      <c r="D3" s="0" t="str">
+      <c r="D3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G214</f>
         <v>~</v>
       </c>
-      <c r="E3" s="0" t="str">
+      <c r="E3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N214</f>
         <v>8 Ohm 2W Speaker 8ohm Round 28mm Loud Speakers Compatible with Small Loudspeaker Audio MP3 MP4 Player Speaker (with Terminal)</v>
       </c>
-      <c r="F3" s="0" t="str">
+      <c r="F3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P214</f>
         <v>Amazon</v>
       </c>
-      <c r="G3" s="0" t="str">
+      <c r="G3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q214</f>
         <v>https://www.amazon.com/dp/B0DCTL83H6</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R214</f>
         <v>0</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S214</f>
         <v>0</v>
       </c>
-      <c r="J3" s="0" t="str">
+      <c r="J3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U214</f>
         <v>ZGW-1</v>
       </c>
-      <c r="K3" s="0" t="str">
+      <c r="K3" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V214</f>
         <v>	YFUSET</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B215</f>
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="str">
+      <c r="B4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C215</f>
         <v>J603</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="C4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D215</f>
         <v>DFPlayermini</v>
       </c>
-      <c r="D4" s="0" t="str">
+      <c r="D4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G215</f>
         <v>https://image.dfrobot.com/image/data/DFR0299/DFPlayer%20Mini%20Manul.pdf</v>
       </c>
-      <c r="E4" s="0" t="str">
+      <c r="E4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N215</f>
         <v>Mini MP3 Player</v>
       </c>
-      <c r="F4" s="0" t="str">
+      <c r="F4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P215</f>
         <v>Amazon</v>
       </c>
-      <c r="G4" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q215</f>
-        <v>Amazon</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" s="11" t="s">
+        <v>672</v>
+      </c>
+      <c r="H4" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R215</f>
         <v>0</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S215</f>
         <v>0</v>
       </c>
-      <c r="J4" s="0" t="str">
+      <c r="J4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U215</f>
         <v>https://www.amazon.com/dp/B089D5NLW1</v>
       </c>
-      <c r="K4" s="0" t="str">
+      <c r="K4" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V215</f>
         <v>DFROBOT</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B216</f>
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="str">
+      <c r="B5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C216</f>
         <v>J701</v>
       </c>
-      <c r="C5" s="0" t="str">
+      <c r="C5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D216</f>
         <v>DE9_Receptacle_MountingHoles</v>
       </c>
-      <c r="D5" s="0" t="str">
+      <c r="D5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G216</f>
         <v> ~</v>
       </c>
-      <c r="E5" s="0" t="str">
+      <c r="E5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N216</f>
         <v>DB9 Male and Female D-Sub Solder Type Connector</v>
       </c>
-      <c r="F5" s="0" t="str">
+      <c r="F5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P216</f>
         <v>Amazon</v>
       </c>
-      <c r="G5" s="0" t="str">
+      <c r="G5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q216</f>
         <v>Amazon</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R216</f>
         <v>0</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S216</f>
         <v>0</v>
       </c>
-      <c r="J5" s="0" t="str">
+      <c r="J5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U216</f>
         <v>https://www.amazon.com/Pc-Accessories-Connectors-Connector-20-Pack/dp/B014IVD7L0/ref=sr_1_1</v>
       </c>
-      <c r="K5" s="0" t="str">
+      <c r="K5" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V216</f>
         <v>Connectors Pro</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B217</f>
         <v>1</v>
       </c>
-      <c r="B6" s="0" t="str">
+      <c r="B6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C217</f>
         <v>SD601</v>
       </c>
-      <c r="C6" s="0" t="str">
+      <c r="C6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D217</f>
         <v>Micro_SD_Card_16GB_DFPLAYER</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G217</f>
         <v>0</v>
       </c>
-      <c r="E6" s="0" t="str">
+      <c r="E6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N217</f>
         <v>SanDisk Flash 16 GB SDHC Flash Memory Card SDSDB-016G </v>
       </c>
-      <c r="F6" s="0" t="str">
+      <c r="F6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P217</f>
         <v>Amazon</v>
       </c>
-      <c r="G6" s="0" t="str">
+      <c r="G6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q217</f>
         <v>https://www.amazon.com/SanDisk-Flash-Memory-SDSDB-016G-Change/dp/B001W1BSM0</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R217</f>
         <v>0</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S217</f>
         <v>0</v>
       </c>
-      <c r="J6" s="0" t="str">
+      <c r="J6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U217</f>
         <v>SDSDB-016G-E11</v>
       </c>
-      <c r="K6" s="0" t="str">
+      <c r="K6" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V217</f>
         <v>	SanDisk</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B218</f>
         <v>1</v>
       </c>
-      <c r="B8" s="0" t="str">
+      <c r="B8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C218</f>
         <v>D105</v>
       </c>
-      <c r="C8" s="0" t="str">
+      <c r="C8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D218</f>
         <v>LED_T1.75_CLEAR_RED</v>
       </c>
-      <c r="D8" s="0" t="str">
+      <c r="D8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G218</f>
         <v>http://optoelectronics.liteon.com/upload/download/DS20-2005-253/LTW-2R3D7.pdf</v>
       </c>
-      <c r="E8" s="0" t="str">
+      <c r="E8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N218</f>
         <v>LED RED CLEAR T-1 3/4 T/H</v>
       </c>
-      <c r="F8" s="0" t="str">
+      <c r="F8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P218</f>
         <v>DigiKey</v>
       </c>
-      <c r="G8" s="0" t="str">
+      <c r="G8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q218</f>
         <v>160-1682-ND</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R218</f>
         <v>0</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S218</f>
         <v>0</v>
       </c>
-      <c r="J8" s="0" t="str">
+      <c r="J8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U218</f>
         <v>LTL2R3KEK</v>
       </c>
-      <c r="K8" s="0" t="str">
+      <c r="K8" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V218</f>
         <v>Lite-On Inc.</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B219</f>
         <v>5</v>
       </c>
-      <c r="B9" s="0" t="str">
+      <c r="B9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C219</f>
         <v>D201, D202, D203, D204, D205</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="C9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D219</f>
         <v>LED_T1.75_CLEAR_WHITE</v>
       </c>
-      <c r="D9" s="0" t="str">
+      <c r="D9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G219</f>
         <v>http://optoelectronics.liteon.com/upload/download/DS20-2005-253/LTW-2R3D7.pdf</v>
       </c>
-      <c r="E9" s="0" t="str">
+      <c r="E9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N219</f>
         <v>LED WHITE CLEAR T-1 3/4 T/H</v>
       </c>
-      <c r="F9" s="0" t="str">
+      <c r="F9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P219</f>
         <v>DigiKey</v>
       </c>
-      <c r="G9" s="0" t="str">
+      <c r="G9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q219</f>
         <v>160-1772-ND</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R219</f>
         <v>0</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S219</f>
         <v>0</v>
       </c>
-      <c r="J9" s="0" t="str">
+      <c r="J9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U219</f>
         <v>LTW-2R3D7</v>
       </c>
-      <c r="K9" s="0" t="str">
+      <c r="K9" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V219</f>
         <v>Lite-On Inc.</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B220</f>
         <v>4</v>
       </c>
-      <c r="B10" s="0" t="str">
+      <c r="B10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C220</f>
         <v>MF403, MF406, MF409, MF412</v>
       </c>
-      <c r="C10" s="0" t="str">
+      <c r="C10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D220</f>
         <v>Nut_4-40_0.1875</v>
       </c>
-      <c r="D10" s="0" t="str">
+      <c r="D10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G220</f>
         <v>https://www.keyelco.com/userAssets/file/M65p135.pdf</v>
       </c>
-      <c r="E10" s="0" t="str">
+      <c r="E10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N220</f>
         <v>#4-40 Hex Nut 0.187" (4.75mm) 3/16" Steel</v>
       </c>
-      <c r="F10" s="0" t="str">
+      <c r="F10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P220</f>
         <v>DigiKey</v>
       </c>
-      <c r="G10" s="0" t="str">
+      <c r="G10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q220</f>
         <v>36-4694-ND</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R220</f>
         <v>0</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S220</f>
         <v>0</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U220</f>
         <v>4694</v>
       </c>
-      <c r="K10" s="0" t="str">
+      <c r="K10" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V220</f>
         <v>Keystone Electronics</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B221</f>
-        <v>4</v>
-      </c>
-      <c r="B12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C221</f>
-        <v>R106, R107, R306, R308</v>
-      </c>
-      <c r="C12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D221</f>
-        <v>DNI</v>
-      </c>
-      <c r="D12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G221</f>
-        <v>~</v>
-      </c>
-      <c r="E12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N221</f>
-        <v>DNI</v>
-      </c>
-      <c r="F12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P221</f>
-        <v>DNI</v>
-      </c>
-      <c r="G12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q221</f>
-        <v>DNI</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R221</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S221</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U221</f>
-        <v>DNI</v>
-      </c>
-      <c r="K12" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V221</f>
-        <v>TyoHM</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A12" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B222</f>
         <v>1</v>
       </c>
-      <c r="B14" s="0" t="str">
+      <c r="B12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C222</f>
         <v>U302</v>
       </c>
-      <c r="C14" s="0" t="str">
+      <c r="C12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D222</f>
         <v>LCD_20x4_Character-GPAD_SCH_LIB</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D12" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G222</f>
         <v>0</v>
       </c>
-      <c r="E14" s="0" t="str">
+      <c r="E12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N222</f>
         <v>2004 LCD Display Module Character 20x4 Blacklight Gray Yellow Blue</v>
       </c>
-      <c r="F14" s="0" t="str">
+      <c r="F12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P222</f>
         <v>eBay   Aliexpress</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q222</f>
         <v>403534100457</v>
       </c>
-      <c r="H14" s="0" t="str">
+      <c r="H12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R222</f>
         <v>Amazon  / Aliexpress</v>
       </c>
-      <c r="I14" s="0" t="str">
+      <c r="I12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S222</f>
         <v>https://www.amazon.com/GeeekPi-Interface-Adapter-Backlight-Raspberry/dp/B07QLRD3TM/ref=sr_1_2 /  https://www.aliexpress.com/item/3256803213374992.html</v>
       </c>
-      <c r="J14" s="0" t="str">
+      <c r="J12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U222</f>
         <v>https://www.ebay.com/itm/403534100457</v>
       </c>
-      <c r="K14" s="0" t="str">
+      <c r="K12" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V222</f>
         <v>NA</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B268</f>
         <v>4</v>
       </c>
-      <c r="B17" s="0" t="str">
+      <c r="B14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C268</f>
         <v>MF401, MF404, MF407, MF410</v>
       </c>
-      <c r="C17" s="0" t="str">
+      <c r="C14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D268</f>
         <v>Screw_4-40_0.375_Phillips</v>
       </c>
-      <c r="D17" s="0" t="str">
+      <c r="D14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G268</f>
         <v>https://www.mcmaster.com/catalog/128/3306</v>
       </c>
-      <c r="E17" s="0" t="str">
+      <c r="E14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N268</f>
         <v>Zinc-Plated Steel Pan Head Phillips Screw, 4-40 Thread, 3/8" Long</v>
       </c>
-      <c r="F17" s="0" t="str">
+      <c r="F14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P268</f>
         <v>McMaster-Carr</v>
       </c>
-      <c r="G17" s="0" t="str">
+      <c r="G14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q268</f>
         <v>90272A108</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H14" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R268</f>
         <v>0</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I14" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S268</f>
         <v>0</v>
       </c>
-      <c r="J17" s="0" t="str">
+      <c r="J14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U268</f>
         <v>90272A108</v>
       </c>
-      <c r="K17" s="0" t="str">
+      <c r="K14" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V268</f>
         <v>McMaster-Carr</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B269</f>
         <v>4</v>
       </c>
-      <c r="B18" s="0" t="str">
+      <c r="B15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C269</f>
         <v>MF402, MF405, MF408, MF411</v>
       </c>
-      <c r="C18" s="0" t="str">
+      <c r="C15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D269</f>
         <v>Spacer_0.0182x0.125 inch</v>
       </c>
-      <c r="D18" s="0" t="str">
+      <c r="D15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G269</f>
         <v>https://www.mcmaster.com/catalog/128/3306</v>
       </c>
-      <c r="E18" s="0" t="str">
+      <c r="E15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N269</f>
         <v>Off-White Nylon Unthreaded Spacer, 0.1875" OD, 1/8" Long, for Number 4 Screw Size</v>
       </c>
-      <c r="F18" s="0" t="str">
+      <c r="F15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P269</f>
         <v>McMaster-Carr</v>
       </c>
-      <c r="G18" s="0" t="str">
+      <c r="G15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q269</f>
         <v>94639A702</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H15" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R269</f>
         <v>0</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I15" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S269</f>
         <v>0</v>
       </c>
-      <c r="J18" s="0" t="str">
+      <c r="J15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U269</f>
         <v>94639A702</v>
       </c>
-      <c r="K18" s="0" t="str">
+      <c r="K15" s="3" t="str">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V269</f>
         <v>McMaster-Carr</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B270</f>
-        <v>4</v>
-      </c>
-      <c r="B20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C270</f>
-        <v>H101, H102, H103, H104</v>
-      </c>
-      <c r="C20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D270</f>
-        <v>MountingHole_Pad_3.5mm</v>
-      </c>
-      <c r="D20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G270</f>
-        <v>~</v>
-      </c>
-      <c r="E20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N270</f>
-        <v>MountingHole_Pad_3.5mm</v>
-      </c>
-      <c r="F20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P270</f>
-        <v>NA</v>
-      </c>
-      <c r="G20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q270</f>
-        <v>NA</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R270</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S270</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U270</f>
-        <v>NA</v>
-      </c>
-      <c r="K20" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V270</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B271</f>
-        <v>6</v>
-      </c>
-      <c r="B21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C271</f>
-        <v>MF103, MF601, MF602, MF603, MF604, MF605</v>
-      </c>
-      <c r="C21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D271</f>
-        <v>U_Box_V104_General_Alarm_Device_LED_Standoff</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G271</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N271</f>
-        <v>NA</v>
-      </c>
-      <c r="F21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P271</f>
-        <v>NA</v>
-      </c>
-      <c r="G21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q271</f>
-        <v>NA</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R271</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S271</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U271</f>
-        <v>NA</v>
-      </c>
-      <c r="K21" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V271</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B272</f>
-        <v>3</v>
-      </c>
-      <c r="B22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C272</f>
-        <v>T101, T102, T103</v>
-      </c>
-      <c r="C22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D272</f>
-        <v>ToolingHole_Pad_1.152mm</v>
-      </c>
-      <c r="D22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G272</f>
-        <v>~</v>
-      </c>
-      <c r="E22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N272</f>
-        <v>ToolingHole_Pad_1.152mm</v>
-      </c>
-      <c r="F22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P272</f>
-        <v>NA</v>
-      </c>
-      <c r="G22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q272</f>
-        <v>NA</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R272</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S272</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U272</f>
-        <v>NA</v>
-      </c>
-      <c r="K22" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V272</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B273</f>
-        <v>1</v>
-      </c>
-      <c r="B24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C273</f>
-        <v>MF801</v>
-      </c>
-      <c r="C24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D273</f>
-        <v>ENCLOSURE_KRAKE_VER1</v>
-      </c>
-      <c r="D24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G273</f>
-        <v>https://www.mcmaster.com/catalog/128/3306</v>
-      </c>
-      <c r="E24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N273</f>
-        <v>NA</v>
-      </c>
-      <c r="F24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P273</f>
-        <v>PublicInvention</v>
-      </c>
-      <c r="G24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q273</f>
-        <v>ENCLOSURE_KRAKE_VER1</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R273</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S273</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U273</f>
-        <v>NA</v>
-      </c>
-      <c r="K24" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V273</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B274</f>
-        <v>1</v>
-      </c>
-      <c r="B25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C274</f>
-        <v>MF802</v>
-      </c>
-      <c r="C25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D274</f>
-        <v>PCB_KRAKE_VER1</v>
-      </c>
-      <c r="D25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G274</f>
-        <v>Gerbers2501181555.zip</v>
-      </c>
-      <c r="E25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N274</f>
-        <v>PCB for KRAKE Version 1</v>
-      </c>
-      <c r="F25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P274</f>
-        <v>PublicInvention</v>
-      </c>
-      <c r="G25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q274</f>
-        <v>PCB_KRAKE_V1</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R274</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S274</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="0" t="str">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U274</f>
-        <v>Gerbers2501181555.zip</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V274</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!B275</f>
         <v>0</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!C275</f>
         <v>0</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!D275</f>
         <v>0</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!G275</f>
         <v>0</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!N275</f>
         <v>0</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!P275</f>
         <v>0</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!Q275</f>
         <v>0</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!R275</f>
         <v>0</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!S275</f>
         <v>0</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!U275</f>
         <v>0</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K17" s="3" t="n">
         <f aca="false">PCBa_KRAKEKiCad6_250128_1359!V275</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" display="https://www.amazon.com/gp/product/B07Y2YKYRS/ref=ox_sc_act_title_1?smid=A39S0U3UP1U7UG&amp;th=1"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>